<commit_message>
uploaded boxplot generation code
</commit_message>
<xml_diff>
--- a/thesis-artifacts/Quantitative Analysis/association_evaluation.xlsx
+++ b/thesis-artifacts/Quantitative Analysis/association_evaluation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rexchou/Desktop/Experiment Data/output/experiment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rexchou/Documents/GitHub/thesis_github/thesis-artifacts/Quantitative Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A41162D-F30E-F24F-94D5-43C1AD8A2C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{757DD3D0-6829-6B40-917A-2A715A0CC8D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="660" windowWidth="25600" windowHeight="14720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -194,17 +194,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,7 +510,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="J12" activeCellId="2" sqref="D12 G12 J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -523,18 +523,18 @@
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
       <c r="E1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
       <c r="H1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -823,7 +823,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B11">
@@ -858,31 +858,31 @@
       <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="3">
         <v>0.754</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>0.78200000000000003</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>0.81899999999999995</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>0.57599999999999996</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>0.56399999999999995</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>0.56599999999999995</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="3">
         <v>0.59</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="3">
         <v>0.623</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="3">
         <v>0.66900000000000004</v>
       </c>
     </row>
@@ -943,15 +943,15 @@
       <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
+      <c r="C1" s="6"/>
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="6"/>
       <c r="F1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
@@ -1185,22 +1185,22 @@
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B12" s="4">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>0.129</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>0.16300000000000001</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>0.105</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>0.14099999999999999</v>
       </c>
     </row>

</xml_diff>